<commit_message>
Update QR generator and emergency app
</commit_message>
<xml_diff>
--- a/inputデータ.xlsx
+++ b/inputデータ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\python\emargencyAPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D129300F-11AF-47CA-8C69-E11B8E38D35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62300B48-92A4-48C9-9E91-E149D1739942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10350" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>nick</t>
   </si>
@@ -33,31 +33,53 @@
     <t>addr</t>
   </si>
   <si>
+    <t>tel</t>
+  </si>
+  <si>
+    <t>おとちゃん</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>りくぼー</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ヒーちゃん</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>千葉市中央区末広４丁目１６－１１</t>
+    <rPh sb="0" eb="3">
+      <t>チバシ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>チュウオウク</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>スエヒロ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>チョウメ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>school</t>
-  </si>
-  <si>
-    <t>tel</t>
-  </si>
-  <si>
-    <t>たろう</t>
-  </si>
-  <si>
-    <t>千葉県市原市…</t>
-  </si>
-  <si>
-    <t>市原第一小学校3年1組</t>
-  </si>
-  <si>
-    <t>090xxxx</t>
-  </si>
-  <si>
-    <t>はなこ</t>
-  </si>
-  <si>
-    <t>市原第一小学校2年2組</t>
-  </si>
-  <si>
-    <t>080xxxx</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>寒川小学校</t>
+    <rPh sb="0" eb="2">
+      <t>サムカワ</t>
+    </rPh>
+    <rPh sb="2" eb="5">
+      <t>ショウガッコウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>09011956792</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -109,12 +131,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -397,16 +422,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="16.75" customWidth="1"/>
+    <col min="2" max="2" width="38.125" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
+    <col min="4" max="4" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -417,38 +444,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>